<commit_message>
Upload excel sheets for working hours
</commit_message>
<xml_diff>
--- a/Sprint1.xlsx
+++ b/Sprint1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\storage\homes\H8244\Dox\Desktop\GitHub\Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\storage\homes\H8244\Dox\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -35,10 +35,10 @@
     <t>Kustannukset AWS-palveluista MTD</t>
   </si>
   <si>
-    <t>https://github.com/DigiaMinions/Project/wiki/TUNTIKIRJAUKSET</t>
+    <t>Tunnit yhteensä 2.1-8.1</t>
   </si>
   <si>
-    <t>Tunnit yhteensä 2.1-8.1</t>
+    <t>https://github.com/DigiaMinions/Project/wiki/Resurssit-ja-ty%C3%B6tunnit</t>
   </si>
 </sst>
 </file>
@@ -374,21 +374,21 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="51.75" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.75" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="70.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="14" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.25" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="28.375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B1">
         <v>4</v>
@@ -422,7 +422,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>